<commit_message>
[UPDATE] Download file tessdata
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="548">
   <si>
     <t>Name</t>
   </si>
@@ -1658,6 +1658,18 @@
   </si>
   <si>
     <t>code_lang</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>link download 4.0</t>
+  </si>
+  <si>
+    <t>.traineddata</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -5080,8 +5092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:DD108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:BD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5421,263 +5433,557 @@
       <c r="D12" s="1" t="s">
         <v>443</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AM12" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AP12" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AR12" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AS12" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AT12" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AU12" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AV12" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AW12" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AX12" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AY12" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AZ12" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="BA12" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="BB12" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="BC12" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="BD12" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="13" spans="4:108" ht="15" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>444</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="14" spans="4:108" ht="15" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
         <v>445</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="15" spans="4:108" ht="15" x14ac:dyDescent="0.2">
       <c r="D15" s="1" t="s">
         <v>446</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="16" spans="4:108" ht="15" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H16" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H17" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="19" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H18" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="20" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H19" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D20" s="1" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="21" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H20" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D21" s="1" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="22" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H21" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D22" s="1" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="23" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H22" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D23" s="1" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="24" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H23" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D24" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="25" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H24" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="26" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H25" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D26" s="1" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="27" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H26" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D27" s="1" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="28" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H27" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D28" s="1" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="29" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H28" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D29" s="1" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="30" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H29" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D30" s="1" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="31" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H30" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D31" s="1" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="32" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H31" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H32" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H33" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H34" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D35" s="1" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H35" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D36" s="1" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="37" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H36" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D37" s="1" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="38" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H37" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D38" s="1" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="39" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H38" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="40" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H39" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D40" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="41" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H40" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D41" s="1" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="42" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H41" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D42" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="43" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H42" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D43" s="1" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="44" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H43" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D44" s="1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="45" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H44" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="45" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D45" s="1" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="46" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H45" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D46" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="47" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H46" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="47" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D47" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="48" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H47" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="48" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D48" s="1" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="49" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H48" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D49" s="1" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="50" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H49" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D50" s="1" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="51" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H50" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D51" s="1" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="52" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H51" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D52" s="1" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="53" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H52" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D53" s="1" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="54" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H53" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D54" s="1" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="55" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H54" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D55" s="1" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="56" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H55" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D56" s="1" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="57" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H56" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D57" s="1" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="58" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H57" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="58" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D58" s="1" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="59" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H58" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="59" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D59" s="1" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="60" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H59" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D60" s="1" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="61" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H60" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D61" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="62" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="H61" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D62" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="63" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D63" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="64" spans="4:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:8" ht="15" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
         <v>495</v>
       </c>
@@ -5904,15 +6210,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:N56"/>
+  <dimension ref="D5:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E56"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8:R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5920,8 +6227,8 @@
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
         <v>378</v>
       </c>
@@ -5937,8 +6244,14 @@
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P6" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D7" s="5" t="s">
         <v>0</v>
       </c>
@@ -5964,8 +6277,18 @@
       <c r="N7" s="7" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P7" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D8" s="5" t="s">
         <v>2</v>
       </c>
@@ -5994,8 +6317,20 @@
         <f>G8</f>
         <v>amh</v>
       </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P8" s="5" t="str">
+        <f>G8</f>
+        <v>amh</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R8" s="6" t="str">
+        <f>CONCATENATE(P8,Q8)</f>
+        <v>amh.traineddata</v>
+      </c>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
@@ -6024,8 +6359,20 @@
         <f t="shared" ref="N9:N56" si="2">G9</f>
         <v>ara</v>
       </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P9" s="5" t="str">
+        <f t="shared" ref="P9:P56" si="3">G9</f>
+        <v>ara</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R9" s="6" t="str">
+        <f t="shared" ref="R9:R56" si="4">CONCATENATE(P9,Q9)</f>
+        <v>ara.traineddata</v>
+      </c>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
@@ -6054,8 +6401,20 @@
         <f t="shared" si="2"/>
         <v>ben</v>
       </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P10" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>ben</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R10" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>ben.traineddata</v>
+      </c>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
@@ -6084,8 +6443,20 @@
         <f t="shared" si="2"/>
         <v>eng</v>
       </c>
-    </row>
-    <row r="12" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P11" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>eng</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R11" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>eng.traineddata</v>
+      </c>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
@@ -6114,8 +6485,20 @@
         <f t="shared" si="2"/>
         <v>por</v>
       </c>
-    </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P12" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>por</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R12" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>por.traineddata</v>
+      </c>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
@@ -6144,8 +6527,20 @@
         <f t="shared" si="2"/>
         <v>bul</v>
       </c>
-    </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P13" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>bul</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R13" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>bul.traineddata</v>
+      </c>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
@@ -6174,8 +6569,20 @@
         <f t="shared" si="2"/>
         <v>cat</v>
       </c>
-    </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P14" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>cat</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R14" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>cat.traineddata</v>
+      </c>
+      <c r="S14" s="7"/>
+    </row>
+    <row r="15" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
@@ -6204,8 +6611,20 @@
         <f t="shared" si="2"/>
         <v>chr</v>
       </c>
-    </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P15" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>chr</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R15" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>chr.traineddata</v>
+      </c>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D16" s="5" t="s">
         <v>84</v>
       </c>
@@ -6234,8 +6653,20 @@
         <f t="shared" si="2"/>
         <v>chi_sim</v>
       </c>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P16" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>chi_sim</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R16" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>chi_sim.traineddata</v>
+      </c>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D17" s="5" t="s">
         <v>102</v>
       </c>
@@ -6264,8 +6695,20 @@
         <f t="shared" si="2"/>
         <v>chi_tra</v>
       </c>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P17" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>chi_tra</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R17" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>chi_tra.traineddata</v>
+      </c>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
@@ -6283,7 +6726,7 @@
       </c>
       <c r="J18" s="7"/>
       <c r="L18" s="5" t="str">
-        <f t="shared" ref="L18:L56" si="3">D18</f>
+        <f t="shared" ref="L18:L56" si="5">D18</f>
         <v>Danish</v>
       </c>
       <c r="M18" s="6" t="str">
@@ -6294,8 +6737,20 @@
         <f t="shared" si="2"/>
         <v>dan</v>
       </c>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P18" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>dan</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R18" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>dan.traineddata</v>
+      </c>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D19" s="5" t="s">
         <v>30</v>
       </c>
@@ -6313,7 +6768,7 @@
       </c>
       <c r="J19" s="7"/>
       <c r="L19" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Estonian</v>
       </c>
       <c r="M19" s="6" t="str">
@@ -6324,8 +6779,20 @@
         <f t="shared" si="2"/>
         <v>est</v>
       </c>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P19" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>est</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R19" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>est.traineddata</v>
+      </c>
+      <c r="S19" s="7"/>
+    </row>
+    <row r="20" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D20" s="5" t="s">
         <v>34</v>
       </c>
@@ -6343,7 +6810,7 @@
       </c>
       <c r="J20" s="7"/>
       <c r="L20" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Finnish</v>
       </c>
       <c r="M20" s="6" t="str">
@@ -6354,8 +6821,20 @@
         <f t="shared" si="2"/>
         <v>fin</v>
       </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P20" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>fin</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R20" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>fin.traineddata</v>
+      </c>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="21" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D21" s="5" t="s">
         <v>36</v>
       </c>
@@ -6373,7 +6852,7 @@
       </c>
       <c r="J21" s="7"/>
       <c r="L21" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>French</v>
       </c>
       <c r="M21" s="6" t="str">
@@ -6384,8 +6863,20 @@
         <f t="shared" si="2"/>
         <v>fra</v>
       </c>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P21" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>fra</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R21" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>fra.traineddata</v>
+      </c>
+      <c r="S21" s="7"/>
+    </row>
+    <row r="22" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D22" s="5" t="s">
         <v>38</v>
       </c>
@@ -6403,7 +6894,7 @@
       </c>
       <c r="J22" s="7"/>
       <c r="L22" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>German</v>
       </c>
       <c r="M22" s="6" t="str">
@@ -6414,8 +6905,20 @@
         <f t="shared" si="2"/>
         <v>frk</v>
       </c>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P22" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>frk</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R22" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>frk.traineddata</v>
+      </c>
+      <c r="S22" s="7"/>
+    </row>
+    <row r="23" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D23" s="5" t="s">
         <v>40</v>
       </c>
@@ -6433,7 +6936,7 @@
       </c>
       <c r="J23" s="7"/>
       <c r="L23" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Greek</v>
       </c>
       <c r="M23" s="6" t="str">
@@ -6444,8 +6947,20 @@
         <f t="shared" si="2"/>
         <v>grc</v>
       </c>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P23" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>grc</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R23" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>grc.traineddata</v>
+      </c>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D24" s="5" t="s">
         <v>42</v>
       </c>
@@ -6463,7 +6978,7 @@
       </c>
       <c r="J24" s="7"/>
       <c r="L24" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Gujarati</v>
       </c>
       <c r="M24" s="6" t="str">
@@ -6474,8 +6989,20 @@
         <f t="shared" si="2"/>
         <v>guj</v>
       </c>
-    </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P24" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>guj</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R24" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>guj.traineddata</v>
+      </c>
+      <c r="S24" s="7"/>
+    </row>
+    <row r="25" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D25" s="5" t="s">
         <v>44</v>
       </c>
@@ -6493,7 +7020,7 @@
       </c>
       <c r="J25" s="7"/>
       <c r="L25" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Hebrew</v>
       </c>
       <c r="M25" s="6" t="str">
@@ -6504,8 +7031,20 @@
         <f t="shared" si="2"/>
         <v>heb</v>
       </c>
-    </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P25" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>heb</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R25" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>heb.traineddata</v>
+      </c>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D26" s="5" t="s">
         <v>46</v>
       </c>
@@ -6523,7 +7062,7 @@
       </c>
       <c r="J26" s="7"/>
       <c r="L26" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Hindi</v>
       </c>
       <c r="M26" s="6" t="str">
@@ -6534,8 +7073,20 @@
         <f t="shared" si="2"/>
         <v>hin</v>
       </c>
-    </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P26" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>hin</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R26" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>hin.traineddata</v>
+      </c>
+      <c r="S26" s="7"/>
+    </row>
+    <row r="27" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D27" s="5" t="s">
         <v>48</v>
       </c>
@@ -6553,7 +7104,7 @@
       </c>
       <c r="J27" s="7"/>
       <c r="L27" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Hungarian</v>
       </c>
       <c r="M27" s="6" t="str">
@@ -6564,8 +7115,20 @@
         <f t="shared" si="2"/>
         <v>hun</v>
       </c>
-    </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P27" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>hun</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R27" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>hun.traineddata</v>
+      </c>
+      <c r="S27" s="7"/>
+    </row>
+    <row r="28" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
@@ -6583,7 +7146,7 @@
       </c>
       <c r="J28" s="7"/>
       <c r="L28" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Icelandic</v>
       </c>
       <c r="M28" s="6" t="str">
@@ -6594,8 +7157,20 @@
         <f t="shared" si="2"/>
         <v>isl</v>
       </c>
-    </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P28" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>isl</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R28" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>isl.traineddata</v>
+      </c>
+      <c r="S28" s="7"/>
+    </row>
+    <row r="29" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D29" s="5" t="s">
         <v>52</v>
       </c>
@@ -6613,7 +7188,7 @@
       </c>
       <c r="J29" s="7"/>
       <c r="L29" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Indonesian</v>
       </c>
       <c r="M29" s="6" t="str">
@@ -6624,8 +7199,20 @@
         <f t="shared" si="2"/>
         <v>ind</v>
       </c>
-    </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P29" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>ind</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R29" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>ind.traineddata</v>
+      </c>
+      <c r="S29" s="7"/>
+    </row>
+    <row r="30" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D30" s="5" t="s">
         <v>54</v>
       </c>
@@ -6643,7 +7230,7 @@
       </c>
       <c r="J30" s="7"/>
       <c r="L30" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Italian</v>
       </c>
       <c r="M30" s="6" t="str">
@@ -6654,8 +7241,20 @@
         <f t="shared" si="2"/>
         <v>ita</v>
       </c>
-    </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P30" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>ita</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R30" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>ita.traineddata</v>
+      </c>
+      <c r="S30" s="7"/>
+    </row>
+    <row r="31" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D31" s="5" t="s">
         <v>56</v>
       </c>
@@ -6673,7 +7272,7 @@
       </c>
       <c r="J31" s="7"/>
       <c r="L31" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Japanese</v>
       </c>
       <c r="M31" s="6" t="str">
@@ -6684,8 +7283,20 @@
         <f t="shared" si="2"/>
         <v>jpn</v>
       </c>
-    </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P31" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>jpn</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R31" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>jpn.traineddata</v>
+      </c>
+      <c r="S31" s="7"/>
+    </row>
+    <row r="32" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D32" s="5" t="s">
         <v>58</v>
       </c>
@@ -6703,7 +7314,7 @@
       </c>
       <c r="J32" s="7"/>
       <c r="L32" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Kannada</v>
       </c>
       <c r="M32" s="6" t="str">
@@ -6714,8 +7325,20 @@
         <f t="shared" si="2"/>
         <v>kan</v>
       </c>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P32" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>kan</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R32" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>kan.traineddata</v>
+      </c>
+      <c r="S32" s="7"/>
+    </row>
+    <row r="33" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D33" s="5" t="s">
         <v>60</v>
       </c>
@@ -6733,7 +7356,7 @@
       </c>
       <c r="J33" s="7"/>
       <c r="L33" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Korean</v>
       </c>
       <c r="M33" s="6" t="str">
@@ -6744,8 +7367,20 @@
         <f t="shared" si="2"/>
         <v>kor</v>
       </c>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P33" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>kor</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R33" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>kor.traineddata</v>
+      </c>
+      <c r="S33" s="7"/>
+    </row>
+    <row r="34" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D34" s="5" t="s">
         <v>62</v>
       </c>
@@ -6763,7 +7398,7 @@
       </c>
       <c r="J34" s="7"/>
       <c r="L34" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Latvian</v>
       </c>
       <c r="M34" s="6" t="str">
@@ -6774,8 +7409,20 @@
         <f t="shared" si="2"/>
         <v>lav</v>
       </c>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P34" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>lav</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R34" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>lav.traineddata</v>
+      </c>
+      <c r="S34" s="7"/>
+    </row>
+    <row r="35" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D35" s="5" t="s">
         <v>64</v>
       </c>
@@ -6793,7 +7440,7 @@
       </c>
       <c r="J35" s="7"/>
       <c r="L35" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Lithuanian</v>
       </c>
       <c r="M35" s="6" t="str">
@@ -6804,8 +7451,20 @@
         <f t="shared" si="2"/>
         <v>lit</v>
       </c>
-    </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P35" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>lit</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R35" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>lit.traineddata</v>
+      </c>
+      <c r="S35" s="7"/>
+    </row>
+    <row r="36" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D36" s="5" t="s">
         <v>66</v>
       </c>
@@ -6823,7 +7482,7 @@
       </c>
       <c r="J36" s="7"/>
       <c r="L36" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Malay</v>
       </c>
       <c r="M36" s="6" t="str">
@@ -6834,8 +7493,20 @@
         <f t="shared" si="2"/>
         <v>msa</v>
       </c>
-    </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P36" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>msa</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R36" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>msa.traineddata</v>
+      </c>
+      <c r="S36" s="7"/>
+    </row>
+    <row r="37" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D37" s="5" t="s">
         <v>68</v>
       </c>
@@ -6853,7 +7524,7 @@
       </c>
       <c r="J37" s="7"/>
       <c r="L37" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Malayalam</v>
       </c>
       <c r="M37" s="6" t="str">
@@ -6864,8 +7535,20 @@
         <f t="shared" si="2"/>
         <v>mal</v>
       </c>
-    </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P37" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>mal</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R37" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>mal.traineddata</v>
+      </c>
+      <c r="S37" s="7"/>
+    </row>
+    <row r="38" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D38" s="5" t="s">
         <v>70</v>
       </c>
@@ -6883,7 +7566,7 @@
       </c>
       <c r="J38" s="7"/>
       <c r="L38" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Marathi</v>
       </c>
       <c r="M38" s="6" t="str">
@@ -6894,8 +7577,20 @@
         <f t="shared" si="2"/>
         <v>mar</v>
       </c>
-    </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P38" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>mar</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R38" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>mar.traineddata</v>
+      </c>
+      <c r="S38" s="7"/>
+    </row>
+    <row r="39" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D39" s="5" t="s">
         <v>72</v>
       </c>
@@ -6913,7 +7608,7 @@
       </c>
       <c r="J39" s="7"/>
       <c r="L39" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Norwegian</v>
       </c>
       <c r="M39" s="6" t="str">
@@ -6924,8 +7619,20 @@
         <f t="shared" si="2"/>
         <v>nor</v>
       </c>
-    </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P39" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>nor</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R39" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>nor.traineddata</v>
+      </c>
+      <c r="S39" s="7"/>
+    </row>
+    <row r="40" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D40" s="5" t="s">
         <v>74</v>
       </c>
@@ -6943,7 +7650,7 @@
       </c>
       <c r="J40" s="7"/>
       <c r="L40" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Polish</v>
       </c>
       <c r="M40" s="6" t="str">
@@ -6954,8 +7661,20 @@
         <f t="shared" si="2"/>
         <v>pol</v>
       </c>
-    </row>
-    <row r="41" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P40" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>pol</v>
+      </c>
+      <c r="Q40" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R40" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>pol.traineddata</v>
+      </c>
+      <c r="S40" s="7"/>
+    </row>
+    <row r="41" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D41" s="5" t="s">
         <v>78</v>
       </c>
@@ -6973,7 +7692,7 @@
       </c>
       <c r="J41" s="7"/>
       <c r="L41" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Romanian</v>
       </c>
       <c r="M41" s="6" t="str">
@@ -6984,8 +7703,20 @@
         <f t="shared" si="2"/>
         <v>ron</v>
       </c>
-    </row>
-    <row r="42" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P41" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>ron</v>
+      </c>
+      <c r="Q41" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R41" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>ron.traineddata</v>
+      </c>
+      <c r="S41" s="7"/>
+    </row>
+    <row r="42" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D42" s="5" t="s">
         <v>80</v>
       </c>
@@ -7003,7 +7734,7 @@
       </c>
       <c r="J42" s="7"/>
       <c r="L42" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Russian</v>
       </c>
       <c r="M42" s="6" t="str">
@@ -7014,8 +7745,20 @@
         <f t="shared" si="2"/>
         <v>rus</v>
       </c>
-    </row>
-    <row r="43" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P42" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>rus</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R42" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>rus.traineddata</v>
+      </c>
+      <c r="S42" s="7"/>
+    </row>
+    <row r="43" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D43" s="5" t="s">
         <v>82</v>
       </c>
@@ -7033,7 +7776,7 @@
       </c>
       <c r="J43" s="7"/>
       <c r="L43" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Serbian</v>
       </c>
       <c r="M43" s="6" t="str">
@@ -7044,8 +7787,20 @@
         <f t="shared" si="2"/>
         <v>srp</v>
       </c>
-    </row>
-    <row r="44" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P43" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>srp</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R43" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>srp.traineddata</v>
+      </c>
+      <c r="S43" s="7"/>
+    </row>
+    <row r="44" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D44" s="5" t="s">
         <v>86</v>
       </c>
@@ -7063,7 +7818,7 @@
       </c>
       <c r="J44" s="7"/>
       <c r="L44" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Slovak</v>
       </c>
       <c r="M44" s="6" t="str">
@@ -7074,8 +7829,20 @@
         <f t="shared" si="2"/>
         <v>slk</v>
       </c>
-    </row>
-    <row r="45" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P44" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>slk</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R44" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>slk.traineddata</v>
+      </c>
+      <c r="S44" s="7"/>
+    </row>
+    <row r="45" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D45" s="5" t="s">
         <v>88</v>
       </c>
@@ -7093,7 +7860,7 @@
       </c>
       <c r="J45" s="7"/>
       <c r="L45" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Slovenian</v>
       </c>
       <c r="M45" s="6" t="str">
@@ -7104,8 +7871,20 @@
         <f t="shared" si="2"/>
         <v>slv</v>
       </c>
-    </row>
-    <row r="46" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P45" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>slv</v>
+      </c>
+      <c r="Q45" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R45" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>slv.traineddata</v>
+      </c>
+      <c r="S45" s="7"/>
+    </row>
+    <row r="46" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D46" s="5" t="s">
         <v>90</v>
       </c>
@@ -7123,7 +7902,7 @@
       </c>
       <c r="J46" s="7"/>
       <c r="L46" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Spanish</v>
       </c>
       <c r="M46" s="6" t="str">
@@ -7134,8 +7913,20 @@
         <f t="shared" si="2"/>
         <v>spa</v>
       </c>
-    </row>
-    <row r="47" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P46" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>spa</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R46" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>spa.traineddata</v>
+      </c>
+      <c r="S46" s="7"/>
+    </row>
+    <row r="47" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D47" s="5" t="s">
         <v>92</v>
       </c>
@@ -7153,7 +7944,7 @@
       </c>
       <c r="J47" s="7"/>
       <c r="L47" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Swahili</v>
       </c>
       <c r="M47" s="6" t="str">
@@ -7164,8 +7955,20 @@
         <f t="shared" si="2"/>
         <v>swa</v>
       </c>
-    </row>
-    <row r="48" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P47" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>swa</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R47" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>swa.traineddata</v>
+      </c>
+      <c r="S47" s="7"/>
+    </row>
+    <row r="48" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D48" s="5" t="s">
         <v>94</v>
       </c>
@@ -7183,7 +7986,7 @@
       </c>
       <c r="J48" s="7"/>
       <c r="L48" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Swedish</v>
       </c>
       <c r="M48" s="6" t="str">
@@ -7194,8 +7997,20 @@
         <f t="shared" si="2"/>
         <v>swe</v>
       </c>
-    </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P48" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>swe</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R48" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>swe.traineddata</v>
+      </c>
+      <c r="S48" s="7"/>
+    </row>
+    <row r="49" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D49" s="5" t="s">
         <v>96</v>
       </c>
@@ -7213,7 +8028,7 @@
       </c>
       <c r="J49" s="7"/>
       <c r="L49" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Tamil</v>
       </c>
       <c r="M49" s="6" t="str">
@@ -7224,8 +8039,20 @@
         <f t="shared" si="2"/>
         <v>tam</v>
       </c>
-    </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P49" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>tam</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R49" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>tam.traineddata</v>
+      </c>
+      <c r="S49" s="7"/>
+    </row>
+    <row r="50" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D50" s="5" t="s">
         <v>98</v>
       </c>
@@ -7243,7 +8070,7 @@
       </c>
       <c r="J50" s="7"/>
       <c r="L50" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Telugu</v>
       </c>
       <c r="M50" s="6" t="str">
@@ -7254,8 +8081,20 @@
         <f t="shared" si="2"/>
         <v>tel</v>
       </c>
-    </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P50" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>tel</v>
+      </c>
+      <c r="Q50" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R50" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>tel.traineddata</v>
+      </c>
+      <c r="S50" s="7"/>
+    </row>
+    <row r="51" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D51" s="5" t="s">
         <v>100</v>
       </c>
@@ -7273,7 +8112,7 @@
       </c>
       <c r="J51" s="7"/>
       <c r="L51" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Thai</v>
       </c>
       <c r="M51" s="6" t="str">
@@ -7284,8 +8123,20 @@
         <f t="shared" si="2"/>
         <v>tha</v>
       </c>
-    </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P51" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>tha</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R51" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>tha.traineddata</v>
+      </c>
+      <c r="S51" s="7"/>
+    </row>
+    <row r="52" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D52" s="5" t="s">
         <v>104</v>
       </c>
@@ -7303,7 +8154,7 @@
       </c>
       <c r="J52" s="7"/>
       <c r="L52" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Turkish</v>
       </c>
       <c r="M52" s="6" t="str">
@@ -7314,8 +8165,20 @@
         <f t="shared" si="2"/>
         <v>tur</v>
       </c>
-    </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P52" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>tur</v>
+      </c>
+      <c r="Q52" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R52" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>tur.traineddata</v>
+      </c>
+      <c r="S52" s="7"/>
+    </row>
+    <row r="53" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D53" s="5" t="s">
         <v>106</v>
       </c>
@@ -7333,7 +8196,7 @@
       </c>
       <c r="J53" s="7"/>
       <c r="L53" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Urdu</v>
       </c>
       <c r="M53" s="6" t="str">
@@ -7344,8 +8207,20 @@
         <f t="shared" si="2"/>
         <v>urd</v>
       </c>
-    </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P53" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>urd</v>
+      </c>
+      <c r="Q53" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R53" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>urd.traineddata</v>
+      </c>
+      <c r="S53" s="7"/>
+    </row>
+    <row r="54" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D54" s="5" t="s">
         <v>108</v>
       </c>
@@ -7363,7 +8238,7 @@
       </c>
       <c r="J54" s="7"/>
       <c r="L54" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Ukrainian</v>
       </c>
       <c r="M54" s="6" t="str">
@@ -7374,8 +8249,20 @@
         <f t="shared" si="2"/>
         <v>ukr</v>
       </c>
-    </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="P54" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>ukr</v>
+      </c>
+      <c r="Q54" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R54" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>ukr.traineddata</v>
+      </c>
+      <c r="S54" s="7"/>
+    </row>
+    <row r="55" spans="4:19" x14ac:dyDescent="0.2">
       <c r="D55" s="5" t="s">
         <v>110</v>
       </c>
@@ -7393,7 +8280,7 @@
       </c>
       <c r="J55" s="7"/>
       <c r="L55" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Vietnamese</v>
       </c>
       <c r="M55" s="6" t="str">
@@ -7404,8 +8291,20 @@
         <f t="shared" si="2"/>
         <v>vie</v>
       </c>
-    </row>
-    <row r="56" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P55" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>vie</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="R55" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>vie.traineddata</v>
+      </c>
+      <c r="S55" s="7"/>
+    </row>
+    <row r="56" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D56" s="8" t="s">
         <v>112</v>
       </c>
@@ -7423,7 +8322,7 @@
       </c>
       <c r="J56" s="10"/>
       <c r="L56" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Welsh</v>
       </c>
       <c r="M56" s="9" t="str">
@@ -7434,6 +8333,18 @@
         <f t="shared" si="2"/>
         <v>cym</v>
       </c>
+      <c r="P56" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>cym</v>
+      </c>
+      <c r="Q56" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="R56" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>cym.traineddata</v>
+      </c>
+      <c r="S56" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>